<commit_message>
fix import excel, and bug save data with ajax
</commit_message>
<xml_diff>
--- a/assets/excel/Data Master.xlsx
+++ b/assets/excel/Data Master.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="161">
   <si>
     <t>ID Master</t>
   </si>
@@ -55,11 +55,14 @@
     <t>ASCO</t>
   </si>
   <si>
+    <t>DISTRIBUTOR</t>
+  </si>
+  <si>
+    <t>ATOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">DISTRIBUTOR
 </t>
-  </si>
-  <si>
-    <t>ATOS</t>
   </si>
   <si>
     <t>AVENTICS</t>
@@ -967,7 +970,7 @@
         <v>1.5</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -975,7 +978,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1.5</v>
@@ -987,7 +990,7 @@
         <v>1.7</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -995,7 +998,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1.5</v>
@@ -1007,7 +1010,7 @@
         <v>1.5</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1015,7 +1018,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>1.5</v>
@@ -1027,7 +1030,7 @@
         <v>1.5</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1035,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>1.5</v>
@@ -1055,7 +1058,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1.5</v>
@@ -1075,7 +1078,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>1.6</v>
@@ -1087,7 +1090,7 @@
         <v>1.8</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1095,7 +1098,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>1.5</v>
@@ -1107,7 +1110,7 @@
         <v>1.7</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1115,7 +1118,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>1.5</v>
@@ -1127,7 +1130,7 @@
         <v>1.5</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1135,7 +1138,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>1.8</v>
@@ -1147,7 +1150,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1155,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>1.3</v>
@@ -1167,7 +1170,7 @@
         <v>1.3</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1175,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>1.8</v>
@@ -1187,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1195,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>1.4</v>
@@ -1207,7 +1210,7 @@
         <v>1.6</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1215,7 +1218,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>1.5</v>
@@ -1227,7 +1230,7 @@
         <v>1.7</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1235,7 +1238,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>1.5</v>
@@ -1247,7 +1250,7 @@
         <v>1.5</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1255,7 +1258,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>1.4</v>
@@ -1267,7 +1270,7 @@
         <v>1.6</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1275,7 +1278,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>1.5</v>
@@ -1295,7 +1298,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>1.8</v>
@@ -1307,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1315,7 +1318,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1327,7 +1330,7 @@
         <v>1.5</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1335,7 +1338,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>1.2</v>
@@ -1347,7 +1350,7 @@
         <v>1.2</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1355,7 +1358,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26">
         <v>1.6</v>
@@ -1367,7 +1370,7 @@
         <v>1.8</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1375,7 +1378,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C27">
         <v>1.6</v>
@@ -1395,7 +1398,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C28">
         <v>1.3</v>
@@ -1407,7 +1410,7 @@
         <v>1.3</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1415,7 +1418,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>1.5</v>
@@ -1435,7 +1438,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>1.7</v>
@@ -1455,7 +1458,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>1.8</v>
@@ -1467,7 +1470,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1475,7 +1478,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32">
         <v>1.3</v>
@@ -1487,7 +1490,7 @@
         <v>1.3</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1495,7 +1498,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33">
         <v>1.3</v>
@@ -1507,7 +1510,7 @@
         <v>1.3</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1515,7 +1518,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34">
         <v>1.5</v>
@@ -1527,7 +1530,7 @@
         <v>1.5</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1535,7 +1538,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C35">
         <v>1.5</v>
@@ -1547,7 +1550,7 @@
         <v>1.7</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1555,7 +1558,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36">
         <v>1.7</v>
@@ -1567,7 +1570,7 @@
         <v>1.9</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1575,7 +1578,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37">
         <v>1.5</v>
@@ -1595,7 +1598,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38">
         <v>1.3</v>
@@ -1607,7 +1610,7 @@
         <v>1.3</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1615,7 +1618,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>1.5</v>
@@ -1635,7 +1638,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C40">
         <v>1.3</v>
@@ -1647,7 +1650,7 @@
         <v>1.3</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1655,7 +1658,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>1.3</v>
@@ -1667,7 +1670,7 @@
         <v>1.3</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1675,7 +1678,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42">
         <v>1.6</v>
@@ -1687,7 +1690,7 @@
         <v>1.8</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1695,7 +1698,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>1.5</v>
@@ -1707,7 +1710,7 @@
         <v>1.5</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1715,7 +1718,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C44">
         <v>1.5</v>
@@ -1727,7 +1730,7 @@
         <v>1.5</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1735,7 +1738,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C45">
         <v>1.5</v>
@@ -1747,7 +1750,7 @@
         <v>1.5</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1755,7 +1758,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C46">
         <v>1.5</v>
@@ -1767,7 +1770,7 @@
         <v>1.5</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1775,7 +1778,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C47">
         <v>1.25</v>
@@ -1795,7 +1798,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <v>1.4</v>
@@ -1807,7 +1810,7 @@
         <v>1.6</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1815,7 +1818,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C49">
         <v>1.8</v>
@@ -1835,7 +1838,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C50">
         <v>1.5</v>
@@ -1855,7 +1858,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C51">
         <v>1.8</v>
@@ -1867,7 +1870,7 @@
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1875,7 +1878,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C52">
         <v>1.5</v>
@@ -1895,7 +1898,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C53">
         <v>1.5</v>
@@ -1907,7 +1910,7 @@
         <v>1.5</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1915,7 +1918,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C54">
         <v>1.5</v>
@@ -1927,7 +1930,7 @@
         <v>1.7</v>
       </c>
       <c r="F54" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1935,7 +1938,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C55">
         <v>1.5</v>
@@ -1955,7 +1958,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C56">
         <v>1.5</v>
@@ -1975,7 +1978,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C57">
         <v>1.4</v>
@@ -1995,7 +1998,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C58">
         <v>1.5</v>
@@ -2007,7 +2010,7 @@
         <v>1.5</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2015,7 +2018,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C59">
         <v>1.3</v>
@@ -2027,7 +2030,7 @@
         <v>1.3</v>
       </c>
       <c r="F59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2035,7 +2038,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C60">
         <v>1.5</v>
@@ -2055,7 +2058,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C61">
         <v>1.8</v>
@@ -2067,7 +2070,7 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2075,7 +2078,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C62">
         <v>1.3</v>
@@ -2087,7 +2090,7 @@
         <v>1.3</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2095,7 +2098,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C63">
         <v>1.7</v>
@@ -2107,7 +2110,7 @@
         <v>1.9</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2115,7 +2118,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C64">
         <v>1.8</v>
@@ -2127,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2135,7 +2138,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C65">
         <v>1.3</v>
@@ -2147,7 +2150,7 @@
         <v>1.3</v>
       </c>
       <c r="F65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2155,7 +2158,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C66">
         <v>1.8</v>
@@ -2167,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2175,7 +2178,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C67">
         <v>1.5</v>
@@ -2187,7 +2190,7 @@
         <v>1.7</v>
       </c>
       <c r="F67" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2195,7 +2198,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C68">
         <v>1.3</v>
@@ -2207,7 +2210,7 @@
         <v>1.3</v>
       </c>
       <c r="F68" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2215,7 +2218,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C69">
         <v>1.7</v>
@@ -2227,7 +2230,7 @@
         <v>1.9</v>
       </c>
       <c r="F69" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2235,7 +2238,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C70">
         <v>1.3</v>
@@ -2247,7 +2250,7 @@
         <v>1.3</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2255,7 +2258,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C71">
         <v>1.3</v>
@@ -2267,7 +2270,7 @@
         <v>1.3</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2275,7 +2278,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C72">
         <v>1.6</v>
@@ -2287,7 +2290,7 @@
         <v>1.7</v>
       </c>
       <c r="F72" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2295,7 +2298,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C73">
         <v>1.5</v>
@@ -2307,7 +2310,7 @@
         <v>1.5</v>
       </c>
       <c r="F73" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2315,7 +2318,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C74">
         <v>1.3</v>
@@ -2327,7 +2330,7 @@
         <v>1.3</v>
       </c>
       <c r="F74" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2335,7 +2338,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C75">
         <v>1.8</v>
@@ -2347,7 +2350,7 @@
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2355,7 +2358,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C76">
         <v>1.5</v>
@@ -2367,7 +2370,7 @@
         <v>1.5</v>
       </c>
       <c r="F76" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2375,7 +2378,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C77">
         <v>1.5</v>
@@ -2395,7 +2398,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C78">
         <v>1.5</v>
@@ -2407,7 +2410,7 @@
         <v>1.5</v>
       </c>
       <c r="F78" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2415,7 +2418,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C79">
         <v>1.5</v>
@@ -2435,7 +2438,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C80">
         <v>1.5</v>
@@ -2447,7 +2450,7 @@
         <v>1.5</v>
       </c>
       <c r="F80" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2455,7 +2458,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C81">
         <v>1.3</v>
@@ -2467,7 +2470,7 @@
         <v>1.3</v>
       </c>
       <c r="F81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2475,7 +2478,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C82">
         <v>1.5</v>
@@ -2495,7 +2498,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C83">
         <v>1.8</v>
@@ -2507,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="F83" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2515,7 +2518,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C84">
         <v>1.5</v>
@@ -2527,7 +2530,7 @@
         <v>1.5</v>
       </c>
       <c r="F84" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2535,7 +2538,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C85">
         <v>1.5</v>
@@ -2547,7 +2550,7 @@
         <v>1.7</v>
       </c>
       <c r="F85" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2555,7 +2558,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C86">
         <v>1.4</v>
@@ -2575,7 +2578,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C87">
         <v>1.8</v>
@@ -2587,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2595,7 +2598,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C88">
         <v>1.5</v>
@@ -2607,7 +2610,7 @@
         <v>1.5</v>
       </c>
       <c r="F88" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2615,7 +2618,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C89">
         <v>1.5</v>
@@ -2635,7 +2638,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C90">
         <v>1.5</v>
@@ -2647,7 +2650,7 @@
         <v>1.5</v>
       </c>
       <c r="F90" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2655,7 +2658,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C91">
         <v>1.8</v>
@@ -2667,7 +2670,7 @@
         <v>2</v>
       </c>
       <c r="F91" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2675,7 +2678,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C92">
         <v>1.3</v>
@@ -2695,7 +2698,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C93">
         <v>1.5</v>
@@ -2707,7 +2710,7 @@
         <v>1.7</v>
       </c>
       <c r="F93" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2715,7 +2718,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C94">
         <v>1.4</v>
@@ -2727,7 +2730,7 @@
         <v>1.4</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2735,7 +2738,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C95">
         <v>1.8</v>
@@ -2747,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2755,7 +2758,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C96">
         <v>1.8</v>
@@ -2775,7 +2778,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C97">
         <v>1.8</v>
@@ -2787,7 +2790,7 @@
         <v>2</v>
       </c>
       <c r="F97" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2795,7 +2798,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C98">
         <v>1.8</v>
@@ -2807,7 +2810,7 @@
         <v>2</v>
       </c>
       <c r="F98" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2815,7 +2818,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C99">
         <v>1.3</v>
@@ -2835,7 +2838,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C100">
         <v>1.5</v>
@@ -2847,7 +2850,7 @@
         <v>1.5</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2855,7 +2858,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C101">
         <v>1.5</v>
@@ -2867,7 +2870,7 @@
         <v>1.5</v>
       </c>
       <c r="F101" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2875,7 +2878,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C102">
         <v>1.6</v>
@@ -2887,7 +2890,7 @@
         <v>1.6</v>
       </c>
       <c r="F102" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2895,7 +2898,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C103">
         <v>1.5</v>
@@ -2907,7 +2910,7 @@
         <v>1.5</v>
       </c>
       <c r="F103" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2915,7 +2918,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C104">
         <v>1.4</v>
@@ -2935,7 +2938,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C105">
         <v>1.8</v>
@@ -2947,7 +2950,7 @@
         <v>2</v>
       </c>
       <c r="F105" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2955,7 +2958,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C106">
         <v>1.4</v>
@@ -2975,7 +2978,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C107">
         <v>1.5</v>
@@ -2995,7 +2998,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C108">
         <v>1.4</v>
@@ -3015,7 +3018,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C109">
         <v>1.5</v>
@@ -3035,7 +3038,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C110">
         <v>1.5</v>
@@ -3047,7 +3050,7 @@
         <v>1.5</v>
       </c>
       <c r="F110" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3055,7 +3058,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C111">
         <v>1.5</v>
@@ -3067,7 +3070,7 @@
         <v>1.7</v>
       </c>
       <c r="F111" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3075,7 +3078,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C112">
         <v>1.7</v>
@@ -3087,7 +3090,7 @@
         <v>1.9</v>
       </c>
       <c r="F112" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3095,7 +3098,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C113">
         <v>1.4</v>
@@ -3107,7 +3110,7 @@
         <v>1.6</v>
       </c>
       <c r="F113" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3115,7 +3118,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C114">
         <v>1.5</v>
@@ -3127,7 +3130,7 @@
         <v>1.7</v>
       </c>
       <c r="F114" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3135,7 +3138,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C115">
         <v>1.5</v>
@@ -3147,7 +3150,7 @@
         <v>1.5</v>
       </c>
       <c r="F115" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3155,7 +3158,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C116">
         <v>1.6</v>
@@ -3175,7 +3178,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C117">
         <v>1.8</v>
@@ -3187,7 +3190,7 @@
         <v>2</v>
       </c>
       <c r="F117" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3195,7 +3198,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C118">
         <v>1.57</v>
@@ -3215,7 +3218,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C119">
         <v>1.5</v>
@@ -3227,7 +3230,7 @@
         <v>1.5</v>
       </c>
       <c r="F119" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3235,7 +3238,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C120">
         <v>1.6</v>
@@ -3247,7 +3250,7 @@
         <v>1.8</v>
       </c>
       <c r="F120" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3255,7 +3258,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C121">
         <v>1.5</v>
@@ -3275,7 +3278,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C122">
         <v>1.8</v>
@@ -3287,7 +3290,7 @@
         <v>2</v>
       </c>
       <c r="F122" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3295,7 +3298,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C123">
         <v>1.6</v>
@@ -3315,7 +3318,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C124">
         <v>1.5</v>
@@ -3327,7 +3330,7 @@
         <v>1.5</v>
       </c>
       <c r="F124" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3335,7 +3338,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C125">
         <v>1.5</v>
@@ -3355,7 +3358,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C126">
         <v>1.5</v>
@@ -3367,7 +3370,7 @@
         <v>1.5</v>
       </c>
       <c r="F126" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3375,7 +3378,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C127">
         <v>1.5</v>
@@ -3387,7 +3390,7 @@
         <v>1.7</v>
       </c>
       <c r="F127" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3395,7 +3398,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C128">
         <v>1.5</v>
@@ -3415,7 +3418,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C129">
         <v>1.8</v>
@@ -3427,7 +3430,7 @@
         <v>2</v>
       </c>
       <c r="F129" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3435,7 +3438,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C130">
         <v>1.5</v>
@@ -3455,7 +3458,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C131">
         <v>1.5</v>
@@ -3467,7 +3470,7 @@
         <v>1.5</v>
       </c>
       <c r="F131" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3475,7 +3478,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C132">
         <v>1.5</v>
@@ -3495,7 +3498,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C133">
         <v>1.6</v>
@@ -3507,7 +3510,7 @@
         <v>1.8</v>
       </c>
       <c r="F133" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3515,7 +3518,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C134">
         <v>1.7</v>
@@ -3527,7 +3530,7 @@
         <v>1.9</v>
       </c>
       <c r="F134" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3535,7 +3538,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C135">
         <v>1.5</v>
@@ -3547,7 +3550,7 @@
         <v>1.5</v>
       </c>
       <c r="F135" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3555,7 +3558,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C136">
         <v>1.5</v>
@@ -3567,7 +3570,7 @@
         <v>1.7</v>
       </c>
       <c r="F136" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3575,7 +3578,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C137">
         <v>1.3</v>
@@ -3587,7 +3590,7 @@
         <v>1.3</v>
       </c>
       <c r="F137" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3595,7 +3598,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C138">
         <v>1.4</v>
@@ -3615,7 +3618,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C139">
         <v>1.4</v>
@@ -3627,7 +3630,7 @@
         <v>1.6</v>
       </c>
       <c r="F139" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -3635,7 +3638,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C140">
         <v>1.8</v>
@@ -3647,7 +3650,7 @@
         <v>2</v>
       </c>
       <c r="F140" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -3655,7 +3658,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C141">
         <v>1.5</v>
@@ -3667,7 +3670,7 @@
         <v>1.5</v>
       </c>
       <c r="F141" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -3675,7 +3678,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C142">
         <v>1.3</v>
@@ -3695,7 +3698,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C143">
         <v>1.2</v>
@@ -3715,7 +3718,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C144">
         <v>1.5</v>
@@ -3727,7 +3730,7 @@
         <v>1.5</v>
       </c>
       <c r="F144" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -3735,7 +3738,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C145">
         <v>1.5</v>
@@ -3747,7 +3750,7 @@
         <v>1.5</v>
       </c>
       <c r="F145" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -3755,7 +3758,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C146">
         <v>1.5</v>
@@ -3767,7 +3770,7 @@
         <v>1.5</v>
       </c>
       <c r="F146" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug get id terakhir
</commit_message>
<xml_diff>
--- a/assets/excel/Data Master.xlsx
+++ b/assets/excel/Data Master.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="161">
   <si>
     <t>ID Master</t>
   </si>
@@ -55,11 +55,14 @@
     <t>ASCO</t>
   </si>
   <si>
+    <t>DISTRIBUTOR</t>
+  </si>
+  <si>
+    <t>ATOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">DISTRIBUTOR
 </t>
-  </si>
-  <si>
-    <t>ATOS</t>
   </si>
   <si>
     <t>AVENTICS</t>
@@ -884,7 +887,7 @@
         <v>1.2</v>
       </c>
       <c r="E2">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -967,7 +970,7 @@
         <v>1.5</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -975,7 +978,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1.5</v>
@@ -987,7 +990,7 @@
         <v>1.7</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -995,7 +998,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1.5</v>
@@ -1007,7 +1010,7 @@
         <v>1.5</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1015,7 +1018,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>1.5</v>
@@ -1027,7 +1030,7 @@
         <v>1.5</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1035,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>1.5</v>
@@ -1055,7 +1058,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1.5</v>
@@ -1075,7 +1078,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>1.6</v>
@@ -1087,7 +1090,7 @@
         <v>1.8</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1095,7 +1098,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>1.5</v>
@@ -1107,7 +1110,7 @@
         <v>1.7</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1115,7 +1118,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>1.5</v>
@@ -1127,7 +1130,7 @@
         <v>1.5</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1135,7 +1138,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>1.8</v>
@@ -1147,7 +1150,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1155,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>1.3</v>
@@ -1167,7 +1170,7 @@
         <v>1.3</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1175,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>1.8</v>
@@ -1187,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1195,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>1.4</v>
@@ -1207,7 +1210,7 @@
         <v>1.6</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1215,7 +1218,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>1.5</v>
@@ -1227,7 +1230,7 @@
         <v>1.7</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1235,7 +1238,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>1.5</v>
@@ -1247,7 +1250,7 @@
         <v>1.5</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1255,7 +1258,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>1.4</v>
@@ -1267,7 +1270,7 @@
         <v>1.6</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1275,7 +1278,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>1.5</v>
@@ -1295,7 +1298,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>1.8</v>
@@ -1307,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1315,7 +1318,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1327,7 +1330,7 @@
         <v>1.5</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1335,7 +1338,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>1.2</v>
@@ -1347,7 +1350,7 @@
         <v>1.2</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1355,7 +1358,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26">
         <v>1.6</v>
@@ -1367,7 +1370,7 @@
         <v>1.8</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1375,7 +1378,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C27">
         <v>1.6</v>
@@ -1395,7 +1398,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C28">
         <v>1.3</v>
@@ -1407,7 +1410,7 @@
         <v>1.3</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1415,7 +1418,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>1.5</v>
@@ -1435,7 +1438,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>1.7</v>
@@ -1455,7 +1458,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>1.8</v>
@@ -1467,7 +1470,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1475,7 +1478,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32">
         <v>1.3</v>
@@ -1487,7 +1490,7 @@
         <v>1.3</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1495,7 +1498,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33">
         <v>1.3</v>
@@ -1507,7 +1510,7 @@
         <v>1.3</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1515,7 +1518,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34">
         <v>1.5</v>
@@ -1527,7 +1530,7 @@
         <v>1.5</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1535,7 +1538,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C35">
         <v>1.5</v>
@@ -1547,7 +1550,7 @@
         <v>1.7</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1555,7 +1558,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36">
         <v>1.7</v>
@@ -1567,7 +1570,7 @@
         <v>1.9</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1575,7 +1578,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37">
         <v>1.5</v>
@@ -1595,7 +1598,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38">
         <v>1.3</v>
@@ -1607,7 +1610,7 @@
         <v>1.3</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1615,7 +1618,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>1.5</v>
@@ -1635,7 +1638,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C40">
         <v>1.3</v>
@@ -1647,7 +1650,7 @@
         <v>1.3</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1655,7 +1658,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>1.3</v>
@@ -1667,7 +1670,7 @@
         <v>1.3</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1675,7 +1678,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42">
         <v>1.6</v>
@@ -1687,7 +1690,7 @@
         <v>1.8</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1695,7 +1698,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>1.5</v>
@@ -1707,7 +1710,7 @@
         <v>1.5</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1715,7 +1718,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C44">
         <v>1.5</v>
@@ -1727,7 +1730,7 @@
         <v>1.5</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1735,7 +1738,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C45">
         <v>1.5</v>
@@ -1747,7 +1750,7 @@
         <v>1.5</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1755,7 +1758,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C46">
         <v>1.5</v>
@@ -1767,7 +1770,7 @@
         <v>1.5</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1775,7 +1778,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C47">
         <v>1.25</v>
@@ -1795,7 +1798,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <v>1.4</v>
@@ -1807,7 +1810,7 @@
         <v>1.6</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1815,7 +1818,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C49">
         <v>1.8</v>
@@ -1835,7 +1838,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C50">
         <v>1.5</v>
@@ -1855,7 +1858,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C51">
         <v>1.8</v>
@@ -1867,7 +1870,7 @@
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1875,7 +1878,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C52">
         <v>1.5</v>
@@ -1895,7 +1898,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C53">
         <v>1.5</v>
@@ -1907,7 +1910,7 @@
         <v>1.5</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1915,7 +1918,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C54">
         <v>1.5</v>
@@ -1927,7 +1930,7 @@
         <v>1.7</v>
       </c>
       <c r="F54" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1935,7 +1938,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C55">
         <v>1.5</v>
@@ -1955,7 +1958,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C56">
         <v>1.5</v>
@@ -1975,7 +1978,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C57">
         <v>1.4</v>
@@ -1995,7 +1998,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C58">
         <v>1.5</v>
@@ -2007,7 +2010,7 @@
         <v>1.5</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2015,7 +2018,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C59">
         <v>1.3</v>
@@ -2027,7 +2030,7 @@
         <v>1.3</v>
       </c>
       <c r="F59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2035,7 +2038,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C60">
         <v>1.5</v>
@@ -2055,7 +2058,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C61">
         <v>1.8</v>
@@ -2067,7 +2070,7 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2075,7 +2078,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C62">
         <v>1.3</v>
@@ -2087,7 +2090,7 @@
         <v>1.3</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2095,7 +2098,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C63">
         <v>1.7</v>
@@ -2107,7 +2110,7 @@
         <v>1.9</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2115,7 +2118,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C64">
         <v>1.8</v>
@@ -2127,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2135,7 +2138,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C65">
         <v>1.3</v>
@@ -2147,7 +2150,7 @@
         <v>1.3</v>
       </c>
       <c r="F65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2155,7 +2158,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C66">
         <v>1.8</v>
@@ -2167,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2175,7 +2178,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C67">
         <v>1.5</v>
@@ -2187,7 +2190,7 @@
         <v>1.7</v>
       </c>
       <c r="F67" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2195,7 +2198,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C68">
         <v>1.3</v>
@@ -2207,7 +2210,7 @@
         <v>1.3</v>
       </c>
       <c r="F68" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2215,7 +2218,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C69">
         <v>1.7</v>
@@ -2227,7 +2230,7 @@
         <v>1.9</v>
       </c>
       <c r="F69" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2235,7 +2238,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C70">
         <v>1.3</v>
@@ -2247,7 +2250,7 @@
         <v>1.3</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2255,7 +2258,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C71">
         <v>1.3</v>
@@ -2267,7 +2270,7 @@
         <v>1.3</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2275,7 +2278,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C72">
         <v>1.6</v>
@@ -2287,7 +2290,7 @@
         <v>1.7</v>
       </c>
       <c r="F72" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2295,7 +2298,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C73">
         <v>1.5</v>
@@ -2307,7 +2310,7 @@
         <v>1.5</v>
       </c>
       <c r="F73" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2315,7 +2318,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C74">
         <v>1.3</v>
@@ -2327,7 +2330,7 @@
         <v>1.3</v>
       </c>
       <c r="F74" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2335,7 +2338,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C75">
         <v>1.8</v>
@@ -2347,7 +2350,7 @@
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2355,7 +2358,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C76">
         <v>1.5</v>
@@ -2367,7 +2370,7 @@
         <v>1.5</v>
       </c>
       <c r="F76" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2375,7 +2378,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C77">
         <v>1.5</v>
@@ -2395,7 +2398,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C78">
         <v>1.5</v>
@@ -2407,7 +2410,7 @@
         <v>1.5</v>
       </c>
       <c r="F78" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2415,7 +2418,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C79">
         <v>1.5</v>
@@ -2435,7 +2438,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C80">
         <v>1.5</v>
@@ -2447,7 +2450,7 @@
         <v>1.5</v>
       </c>
       <c r="F80" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2455,7 +2458,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C81">
         <v>1.3</v>
@@ -2467,7 +2470,7 @@
         <v>1.3</v>
       </c>
       <c r="F81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2475,7 +2478,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C82">
         <v>1.5</v>
@@ -2495,7 +2498,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C83">
         <v>1.8</v>
@@ -2507,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="F83" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2515,7 +2518,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C84">
         <v>1.5</v>
@@ -2527,7 +2530,7 @@
         <v>1.5</v>
       </c>
       <c r="F84" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2535,7 +2538,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C85">
         <v>1.5</v>
@@ -2547,7 +2550,7 @@
         <v>1.7</v>
       </c>
       <c r="F85" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2555,7 +2558,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C86">
         <v>1.4</v>
@@ -2575,7 +2578,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C87">
         <v>1.8</v>
@@ -2587,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2595,7 +2598,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C88">
         <v>1.5</v>
@@ -2607,7 +2610,7 @@
         <v>1.5</v>
       </c>
       <c r="F88" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2615,7 +2618,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C89">
         <v>1.5</v>
@@ -2635,7 +2638,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C90">
         <v>1.5</v>
@@ -2647,7 +2650,7 @@
         <v>1.5</v>
       </c>
       <c r="F90" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2655,7 +2658,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C91">
         <v>1.8</v>
@@ -2667,7 +2670,7 @@
         <v>2</v>
       </c>
       <c r="F91" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2675,7 +2678,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C92">
         <v>1.3</v>
@@ -2695,7 +2698,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C93">
         <v>1.5</v>
@@ -2707,7 +2710,7 @@
         <v>1.7</v>
       </c>
       <c r="F93" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2715,7 +2718,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C94">
         <v>1.4</v>
@@ -2727,7 +2730,7 @@
         <v>1.4</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2735,7 +2738,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C95">
         <v>1.8</v>
@@ -2747,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2755,7 +2758,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C96">
         <v>1.8</v>
@@ -2775,7 +2778,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C97">
         <v>1.8</v>
@@ -2787,7 +2790,7 @@
         <v>2</v>
       </c>
       <c r="F97" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2795,7 +2798,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C98">
         <v>1.8</v>
@@ -2807,7 +2810,7 @@
         <v>2</v>
       </c>
       <c r="F98" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2815,7 +2818,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C99">
         <v>1.3</v>
@@ -2835,7 +2838,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C100">
         <v>1.5</v>
@@ -2847,7 +2850,7 @@
         <v>1.5</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2855,7 +2858,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C101">
         <v>1.5</v>
@@ -2867,7 +2870,7 @@
         <v>1.5</v>
       </c>
       <c r="F101" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2875,7 +2878,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C102">
         <v>1.6</v>
@@ -2887,7 +2890,7 @@
         <v>1.6</v>
       </c>
       <c r="F102" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2895,7 +2898,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C103">
         <v>1.5</v>
@@ -2907,7 +2910,7 @@
         <v>1.5</v>
       </c>
       <c r="F103" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2915,7 +2918,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C104">
         <v>1.4</v>
@@ -2935,7 +2938,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C105">
         <v>1.8</v>
@@ -2947,7 +2950,7 @@
         <v>2</v>
       </c>
       <c r="F105" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2955,7 +2958,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C106">
         <v>1.4</v>
@@ -2975,7 +2978,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C107">
         <v>1.5</v>
@@ -2995,7 +2998,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C108">
         <v>1.4</v>
@@ -3015,7 +3018,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C109">
         <v>1.5</v>
@@ -3035,7 +3038,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C110">
         <v>1.5</v>
@@ -3047,7 +3050,7 @@
         <v>1.5</v>
       </c>
       <c r="F110" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3055,7 +3058,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C111">
         <v>1.5</v>
@@ -3067,7 +3070,7 @@
         <v>1.7</v>
       </c>
       <c r="F111" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3075,7 +3078,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C112">
         <v>1.7</v>
@@ -3087,7 +3090,7 @@
         <v>1.9</v>
       </c>
       <c r="F112" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3095,7 +3098,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C113">
         <v>1.4</v>
@@ -3107,7 +3110,7 @@
         <v>1.6</v>
       </c>
       <c r="F113" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3115,7 +3118,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C114">
         <v>1.5</v>
@@ -3127,7 +3130,7 @@
         <v>1.7</v>
       </c>
       <c r="F114" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3135,7 +3138,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C115">
         <v>1.5</v>
@@ -3147,7 +3150,7 @@
         <v>1.5</v>
       </c>
       <c r="F115" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3155,7 +3158,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C116">
         <v>1.6</v>
@@ -3175,7 +3178,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C117">
         <v>1.8</v>
@@ -3187,7 +3190,7 @@
         <v>2</v>
       </c>
       <c r="F117" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3195,7 +3198,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C118">
         <v>1.57</v>
@@ -3215,7 +3218,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C119">
         <v>1.5</v>
@@ -3227,7 +3230,7 @@
         <v>1.5</v>
       </c>
       <c r="F119" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3235,7 +3238,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C120">
         <v>1.6</v>
@@ -3247,7 +3250,7 @@
         <v>1.8</v>
       </c>
       <c r="F120" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3255,7 +3258,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C121">
         <v>1.5</v>
@@ -3275,7 +3278,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C122">
         <v>1.8</v>
@@ -3287,7 +3290,7 @@
         <v>2</v>
       </c>
       <c r="F122" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3295,7 +3298,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C123">
         <v>1.6</v>
@@ -3315,7 +3318,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C124">
         <v>1.5</v>
@@ -3327,7 +3330,7 @@
         <v>1.5</v>
       </c>
       <c r="F124" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3335,7 +3338,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C125">
         <v>1.5</v>
@@ -3355,7 +3358,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C126">
         <v>1.5</v>
@@ -3367,7 +3370,7 @@
         <v>1.5</v>
       </c>
       <c r="F126" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3375,7 +3378,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C127">
         <v>1.5</v>
@@ -3387,7 +3390,7 @@
         <v>1.7</v>
       </c>
       <c r="F127" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3395,7 +3398,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C128">
         <v>1.5</v>
@@ -3415,7 +3418,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C129">
         <v>1.8</v>
@@ -3427,7 +3430,7 @@
         <v>2</v>
       </c>
       <c r="F129" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3435,7 +3438,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C130">
         <v>1.5</v>
@@ -3455,7 +3458,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C131">
         <v>1.5</v>
@@ -3467,7 +3470,7 @@
         <v>1.5</v>
       </c>
       <c r="F131" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3475,7 +3478,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C132">
         <v>1.5</v>
@@ -3495,7 +3498,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C133">
         <v>1.6</v>
@@ -3507,7 +3510,7 @@
         <v>1.8</v>
       </c>
       <c r="F133" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3515,7 +3518,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C134">
         <v>1.7</v>
@@ -3527,7 +3530,7 @@
         <v>1.9</v>
       </c>
       <c r="F134" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3535,7 +3538,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C135">
         <v>1.5</v>
@@ -3547,7 +3550,7 @@
         <v>1.5</v>
       </c>
       <c r="F135" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3555,7 +3558,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C136">
         <v>1.5</v>
@@ -3567,7 +3570,7 @@
         <v>1.7</v>
       </c>
       <c r="F136" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3575,7 +3578,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C137">
         <v>1.3</v>
@@ -3587,7 +3590,7 @@
         <v>1.3</v>
       </c>
       <c r="F137" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3595,7 +3598,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C138">
         <v>1.4</v>
@@ -3615,7 +3618,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C139">
         <v>1.4</v>
@@ -3627,7 +3630,7 @@
         <v>1.6</v>
       </c>
       <c r="F139" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -3635,7 +3638,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C140">
         <v>1.8</v>
@@ -3647,7 +3650,7 @@
         <v>2</v>
       </c>
       <c r="F140" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -3655,7 +3658,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C141">
         <v>1.5</v>
@@ -3667,7 +3670,7 @@
         <v>1.5</v>
       </c>
       <c r="F141" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -3675,7 +3678,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C142">
         <v>1.3</v>
@@ -3695,7 +3698,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C143">
         <v>1.2</v>
@@ -3715,7 +3718,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C144">
         <v>1.5</v>
@@ -3727,7 +3730,7 @@
         <v>1.5</v>
       </c>
       <c r="F144" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -3735,7 +3738,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C145">
         <v>1.5</v>
@@ -3747,7 +3750,7 @@
         <v>1.5</v>
       </c>
       <c r="F145" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -3755,7 +3758,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C146">
         <v>1.5</v>
@@ -3767,7 +3770,7 @@
         <v>1.5</v>
       </c>
       <c r="F146" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix submit button disable after click
</commit_message>
<xml_diff>
--- a/assets/excel/Data Master.xlsx
+++ b/assets/excel/Data Master.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="161">
   <si>
     <t>ID Master</t>
   </si>
@@ -36,15 +36,15 @@
   </si>
   <si>
     <t>AIRTAC</t>
-  </si>
-  <si>
-    <t>ALKITRONIC</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
+    <t>ALKITRONIC</t>
+  </si>
+  <si>
     <t>AOI</t>
   </si>
   <si>
@@ -55,11 +55,14 @@
     <t>ASCO</t>
   </si>
   <si>
+    <t>DISTRIBUTOR</t>
+  </si>
+  <si>
+    <t>ATOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">DISTRIBUTOR
 </t>
-  </si>
-  <si>
-    <t>ATOS</t>
   </si>
   <si>
     <t>AVENTICS</t>
@@ -884,28 +887,30 @@
         <v>1.2</v>
       </c>
       <c r="E2">
-        <v>1.2</v>
-      </c>
-      <c r="F2"/>
+        <v>1.3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3">
-        <v>1.5</v>
-      </c>
-      <c r="D3">
-        <v>1.5</v>
-      </c>
-      <c r="E3">
-        <v>1.5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -965,7 +970,7 @@
         <v>1.5</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -973,7 +978,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1.5</v>
@@ -985,7 +990,7 @@
         <v>1.7</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -993,7 +998,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1.5</v>
@@ -1005,7 +1010,7 @@
         <v>1.5</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1013,7 +1018,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>1.5</v>
@@ -1025,7 +1030,7 @@
         <v>1.5</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1033,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>1.5</v>
@@ -1045,7 +1050,7 @@
         <v>1.5</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1053,7 +1058,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1.5</v>
@@ -1073,7 +1078,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>1.6</v>
@@ -1085,7 +1090,7 @@
         <v>1.8</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1093,7 +1098,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>1.5</v>
@@ -1105,7 +1110,7 @@
         <v>1.7</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1113,7 +1118,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>1.5</v>
@@ -1125,7 +1130,7 @@
         <v>1.5</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1133,7 +1138,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>1.8</v>
@@ -1145,7 +1150,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1153,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>1.3</v>
@@ -1165,7 +1170,7 @@
         <v>1.3</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1173,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>1.8</v>
@@ -1185,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1193,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>1.4</v>
@@ -1205,7 +1210,7 @@
         <v>1.6</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1213,7 +1218,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>1.5</v>
@@ -1225,7 +1230,7 @@
         <v>1.7</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1233,7 +1238,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>1.5</v>
@@ -1245,7 +1250,7 @@
         <v>1.5</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1253,7 +1258,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>1.4</v>
@@ -1265,7 +1270,7 @@
         <v>1.6</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1273,7 +1278,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>1.5</v>
@@ -1293,7 +1298,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>1.8</v>
@@ -1305,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1313,7 +1318,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1325,7 +1330,7 @@
         <v>1.5</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1333,7 +1338,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>1.2</v>
@@ -1345,7 +1350,7 @@
         <v>1.2</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1353,7 +1358,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26">
         <v>1.6</v>
@@ -1365,7 +1370,7 @@
         <v>1.8</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1373,7 +1378,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C27">
         <v>1.6</v>
@@ -1385,7 +1390,7 @@
         <v>1.8</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1393,7 +1398,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C28">
         <v>1.3</v>
@@ -1405,7 +1410,7 @@
         <v>1.3</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1413,7 +1418,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>1.5</v>
@@ -1433,7 +1438,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>1.7</v>
@@ -1445,7 +1450,7 @@
         <v>1.7</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1453,7 +1458,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>1.8</v>
@@ -1465,7 +1470,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1473,7 +1478,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32">
         <v>1.3</v>
@@ -1485,7 +1490,7 @@
         <v>1.3</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1493,7 +1498,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33">
         <v>1.3</v>
@@ -1505,7 +1510,7 @@
         <v>1.3</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1513,7 +1518,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34">
         <v>1.5</v>
@@ -1525,7 +1530,7 @@
         <v>1.5</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1533,7 +1538,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C35">
         <v>1.5</v>
@@ -1545,7 +1550,7 @@
         <v>1.7</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1553,7 +1558,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36">
         <v>1.7</v>
@@ -1565,7 +1570,7 @@
         <v>1.9</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1573,7 +1578,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37">
         <v>1.5</v>
@@ -1585,7 +1590,7 @@
         <v>1.5</v>
       </c>
       <c r="F37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1593,7 +1598,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38">
         <v>1.3</v>
@@ -1605,7 +1610,7 @@
         <v>1.3</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1613,7 +1618,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>1.5</v>
@@ -1625,7 +1630,7 @@
         <v>1.7</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1633,7 +1638,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C40">
         <v>1.3</v>
@@ -1645,7 +1650,7 @@
         <v>1.3</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1653,7 +1658,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>1.3</v>
@@ -1665,7 +1670,7 @@
         <v>1.3</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1673,7 +1678,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42">
         <v>1.6</v>
@@ -1685,7 +1690,7 @@
         <v>1.8</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1693,7 +1698,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>1.5</v>
@@ -1705,7 +1710,7 @@
         <v>1.5</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1713,7 +1718,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C44">
         <v>1.5</v>
@@ -1725,7 +1730,7 @@
         <v>1.5</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1733,7 +1738,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C45">
         <v>1.5</v>
@@ -1745,7 +1750,7 @@
         <v>1.5</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1753,7 +1758,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C46">
         <v>1.5</v>
@@ -1765,7 +1770,7 @@
         <v>1.5</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1773,7 +1778,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C47">
         <v>1.25</v>
@@ -1785,7 +1790,7 @@
         <v>1.25</v>
       </c>
       <c r="F47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1793,7 +1798,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <v>1.4</v>
@@ -1805,7 +1810,7 @@
         <v>1.6</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1813,7 +1818,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C49">
         <v>1.8</v>
@@ -1833,7 +1838,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C50">
         <v>1.5</v>
@@ -1853,7 +1858,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C51">
         <v>1.8</v>
@@ -1865,7 +1870,7 @@
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1873,7 +1878,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C52">
         <v>1.5</v>
@@ -1893,7 +1898,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C53">
         <v>1.5</v>
@@ -1905,7 +1910,7 @@
         <v>1.5</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1913,7 +1918,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C54">
         <v>1.5</v>
@@ -1925,7 +1930,7 @@
         <v>1.7</v>
       </c>
       <c r="F54" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1933,7 +1938,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C55">
         <v>1.5</v>
@@ -1953,7 +1958,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C56">
         <v>1.5</v>
@@ -1965,7 +1970,7 @@
         <v>1.5</v>
       </c>
       <c r="F56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1973,7 +1978,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C57">
         <v>1.4</v>
@@ -1993,7 +1998,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C58">
         <v>1.5</v>
@@ -2005,7 +2010,7 @@
         <v>1.5</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2013,7 +2018,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C59">
         <v>1.3</v>
@@ -2025,7 +2030,7 @@
         <v>1.3</v>
       </c>
       <c r="F59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2033,7 +2038,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C60">
         <v>1.5</v>
@@ -2045,7 +2050,7 @@
         <v>1.5</v>
       </c>
       <c r="F60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2053,7 +2058,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C61">
         <v>1.8</v>
@@ -2065,7 +2070,7 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2073,7 +2078,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C62">
         <v>1.3</v>
@@ -2085,7 +2090,7 @@
         <v>1.3</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2093,7 +2098,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C63">
         <v>1.7</v>
@@ -2105,7 +2110,7 @@
         <v>1.9</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2113,7 +2118,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C64">
         <v>1.8</v>
@@ -2125,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2133,7 +2138,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C65">
         <v>1.3</v>
@@ -2145,7 +2150,7 @@
         <v>1.3</v>
       </c>
       <c r="F65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2153,7 +2158,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C66">
         <v>1.8</v>
@@ -2165,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2173,7 +2178,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C67">
         <v>1.5</v>
@@ -2185,7 +2190,7 @@
         <v>1.7</v>
       </c>
       <c r="F67" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2193,7 +2198,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C68">
         <v>1.3</v>
@@ -2205,7 +2210,7 @@
         <v>1.3</v>
       </c>
       <c r="F68" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2213,7 +2218,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C69">
         <v>1.7</v>
@@ -2225,7 +2230,7 @@
         <v>1.9</v>
       </c>
       <c r="F69" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2233,7 +2238,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C70">
         <v>1.3</v>
@@ -2245,7 +2250,7 @@
         <v>1.3</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2253,7 +2258,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C71">
         <v>1.3</v>
@@ -2265,7 +2270,7 @@
         <v>1.3</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2273,7 +2278,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C72">
         <v>1.6</v>
@@ -2285,7 +2290,7 @@
         <v>1.7</v>
       </c>
       <c r="F72" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2293,7 +2298,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C73">
         <v>1.5</v>
@@ -2305,7 +2310,7 @@
         <v>1.5</v>
       </c>
       <c r="F73" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2313,7 +2318,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C74">
         <v>1.3</v>
@@ -2325,7 +2330,7 @@
         <v>1.3</v>
       </c>
       <c r="F74" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2333,7 +2338,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C75">
         <v>1.8</v>
@@ -2345,7 +2350,7 @@
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2353,7 +2358,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C76">
         <v>1.5</v>
@@ -2365,7 +2370,7 @@
         <v>1.5</v>
       </c>
       <c r="F76" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2373,7 +2378,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C77">
         <v>1.5</v>
@@ -2393,7 +2398,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C78">
         <v>1.5</v>
@@ -2405,7 +2410,7 @@
         <v>1.5</v>
       </c>
       <c r="F78" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2413,7 +2418,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C79">
         <v>1.5</v>
@@ -2433,7 +2438,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C80">
         <v>1.5</v>
@@ -2445,7 +2450,7 @@
         <v>1.5</v>
       </c>
       <c r="F80" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2453,7 +2458,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C81">
         <v>1.3</v>
@@ -2465,7 +2470,7 @@
         <v>1.3</v>
       </c>
       <c r="F81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2473,7 +2478,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C82">
         <v>1.5</v>
@@ -2485,7 +2490,7 @@
         <v>1.5</v>
       </c>
       <c r="F82" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2493,7 +2498,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C83">
         <v>1.8</v>
@@ -2505,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="F83" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2513,7 +2518,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C84">
         <v>1.5</v>
@@ -2525,7 +2530,7 @@
         <v>1.5</v>
       </c>
       <c r="F84" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2533,7 +2538,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C85">
         <v>1.5</v>
@@ -2545,7 +2550,7 @@
         <v>1.7</v>
       </c>
       <c r="F85" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2553,7 +2558,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C86">
         <v>1.4</v>
@@ -2573,7 +2578,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C87">
         <v>1.8</v>
@@ -2585,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2593,7 +2598,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C88">
         <v>1.5</v>
@@ -2605,7 +2610,7 @@
         <v>1.5</v>
       </c>
       <c r="F88" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2613,7 +2618,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C89">
         <v>1.5</v>
@@ -2633,7 +2638,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C90">
         <v>1.5</v>
@@ -2645,7 +2650,7 @@
         <v>1.5</v>
       </c>
       <c r="F90" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2653,7 +2658,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C91">
         <v>1.8</v>
@@ -2665,7 +2670,7 @@
         <v>2</v>
       </c>
       <c r="F91" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2673,7 +2678,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C92">
         <v>1.3</v>
@@ -2693,7 +2698,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C93">
         <v>1.5</v>
@@ -2705,7 +2710,7 @@
         <v>1.7</v>
       </c>
       <c r="F93" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2713,7 +2718,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C94">
         <v>1.4</v>
@@ -2725,7 +2730,7 @@
         <v>1.4</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2733,7 +2738,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C95">
         <v>1.8</v>
@@ -2745,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2753,7 +2758,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C96">
         <v>1.8</v>
@@ -2765,7 +2770,7 @@
         <v>2</v>
       </c>
       <c r="F96" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2773,7 +2778,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C97">
         <v>1.8</v>
@@ -2785,7 +2790,7 @@
         <v>2</v>
       </c>
       <c r="F97" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2793,7 +2798,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C98">
         <v>1.8</v>
@@ -2805,7 +2810,7 @@
         <v>2</v>
       </c>
       <c r="F98" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2813,7 +2818,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C99">
         <v>1.3</v>
@@ -2833,7 +2838,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C100">
         <v>1.5</v>
@@ -2845,7 +2850,7 @@
         <v>1.5</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2853,7 +2858,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C101">
         <v>1.5</v>
@@ -2865,7 +2870,7 @@
         <v>1.5</v>
       </c>
       <c r="F101" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2873,7 +2878,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C102">
         <v>1.6</v>
@@ -2885,7 +2890,7 @@
         <v>1.6</v>
       </c>
       <c r="F102" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2893,7 +2898,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C103">
         <v>1.5</v>
@@ -2905,7 +2910,7 @@
         <v>1.5</v>
       </c>
       <c r="F103" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2913,7 +2918,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C104">
         <v>1.4</v>
@@ -2925,7 +2930,7 @@
         <v>1.6</v>
       </c>
       <c r="F104" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2933,7 +2938,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C105">
         <v>1.8</v>
@@ -2945,7 +2950,7 @@
         <v>2</v>
       </c>
       <c r="F105" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2953,7 +2958,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C106">
         <v>1.4</v>
@@ -2965,7 +2970,7 @@
         <v>1.6</v>
       </c>
       <c r="F106" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2973,7 +2978,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C107">
         <v>1.5</v>
@@ -2985,7 +2990,7 @@
         <v>1.5</v>
       </c>
       <c r="F107" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2993,7 +2998,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C108">
         <v>1.4</v>
@@ -3005,7 +3010,7 @@
         <v>1.6</v>
       </c>
       <c r="F108" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3013,7 +3018,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C109">
         <v>1.5</v>
@@ -3025,7 +3030,7 @@
         <v>1.5</v>
       </c>
       <c r="F109" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3033,7 +3038,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C110">
         <v>1.5</v>
@@ -3045,7 +3050,7 @@
         <v>1.5</v>
       </c>
       <c r="F110" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3053,7 +3058,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C111">
         <v>1.5</v>
@@ -3065,7 +3070,7 @@
         <v>1.7</v>
       </c>
       <c r="F111" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3073,7 +3078,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C112">
         <v>1.7</v>
@@ -3085,7 +3090,7 @@
         <v>1.9</v>
       </c>
       <c r="F112" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3093,7 +3098,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C113">
         <v>1.4</v>
@@ -3105,7 +3110,7 @@
         <v>1.6</v>
       </c>
       <c r="F113" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3113,7 +3118,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C114">
         <v>1.5</v>
@@ -3125,7 +3130,7 @@
         <v>1.7</v>
       </c>
       <c r="F114" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3133,7 +3138,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C115">
         <v>1.5</v>
@@ -3145,7 +3150,7 @@
         <v>1.5</v>
       </c>
       <c r="F115" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3153,7 +3158,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C116">
         <v>1.6</v>
@@ -3173,7 +3178,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C117">
         <v>1.8</v>
@@ -3185,7 +3190,7 @@
         <v>2</v>
       </c>
       <c r="F117" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3193,7 +3198,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C118">
         <v>1.57</v>
@@ -3205,7 +3210,7 @@
         <v>1.57</v>
       </c>
       <c r="F118" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3213,7 +3218,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C119">
         <v>1.5</v>
@@ -3225,7 +3230,7 @@
         <v>1.5</v>
       </c>
       <c r="F119" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3233,7 +3238,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C120">
         <v>1.6</v>
@@ -3245,7 +3250,7 @@
         <v>1.8</v>
       </c>
       <c r="F120" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3253,7 +3258,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C121">
         <v>1.5</v>
@@ -3273,7 +3278,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C122">
         <v>1.8</v>
@@ -3285,7 +3290,7 @@
         <v>2</v>
       </c>
       <c r="F122" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3293,7 +3298,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C123">
         <v>1.6</v>
@@ -3313,7 +3318,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C124">
         <v>1.5</v>
@@ -3325,7 +3330,7 @@
         <v>1.5</v>
       </c>
       <c r="F124" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3333,7 +3338,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C125">
         <v>1.5</v>
@@ -3345,7 +3350,7 @@
         <v>1.5</v>
       </c>
       <c r="F125" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3353,7 +3358,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C126">
         <v>1.5</v>
@@ -3365,7 +3370,7 @@
         <v>1.5</v>
       </c>
       <c r="F126" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3373,7 +3378,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C127">
         <v>1.5</v>
@@ -3385,7 +3390,7 @@
         <v>1.7</v>
       </c>
       <c r="F127" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3393,7 +3398,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C128">
         <v>1.5</v>
@@ -3413,7 +3418,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C129">
         <v>1.8</v>
@@ -3425,7 +3430,7 @@
         <v>2</v>
       </c>
       <c r="F129" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3433,7 +3438,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C130">
         <v>1.5</v>
@@ -3445,7 +3450,7 @@
         <v>1.7</v>
       </c>
       <c r="F130" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3453,7 +3458,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C131">
         <v>1.5</v>
@@ -3465,7 +3470,7 @@
         <v>1.5</v>
       </c>
       <c r="F131" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3473,7 +3478,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C132">
         <v>1.5</v>
@@ -3493,7 +3498,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C133">
         <v>1.6</v>
@@ -3505,7 +3510,7 @@
         <v>1.8</v>
       </c>
       <c r="F133" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3513,7 +3518,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C134">
         <v>1.7</v>
@@ -3525,7 +3530,7 @@
         <v>1.9</v>
       </c>
       <c r="F134" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3533,7 +3538,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C135">
         <v>1.5</v>
@@ -3545,7 +3550,7 @@
         <v>1.5</v>
       </c>
       <c r="F135" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3553,7 +3558,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C136">
         <v>1.5</v>
@@ -3565,7 +3570,7 @@
         <v>1.7</v>
       </c>
       <c r="F136" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3573,7 +3578,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C137">
         <v>1.3</v>
@@ -3585,7 +3590,7 @@
         <v>1.3</v>
       </c>
       <c r="F137" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3593,7 +3598,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C138">
         <v>1.4</v>
@@ -3613,7 +3618,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C139">
         <v>1.4</v>
@@ -3625,7 +3630,7 @@
         <v>1.6</v>
       </c>
       <c r="F139" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -3633,7 +3638,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C140">
         <v>1.8</v>
@@ -3645,7 +3650,7 @@
         <v>2</v>
       </c>
       <c r="F140" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -3653,7 +3658,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C141">
         <v>1.5</v>
@@ -3665,7 +3670,7 @@
         <v>1.5</v>
       </c>
       <c r="F141" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -3673,7 +3678,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C142">
         <v>1.3</v>
@@ -3685,7 +3690,7 @@
         <v>1.3</v>
       </c>
       <c r="F142" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -3693,7 +3698,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C143">
         <v>1.2</v>
@@ -3705,7 +3710,7 @@
         <v>1.2</v>
       </c>
       <c r="F143" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -3713,7 +3718,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C144">
         <v>1.5</v>
@@ -3725,7 +3730,7 @@
         <v>1.5</v>
       </c>
       <c r="F144" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -3733,7 +3738,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C145">
         <v>1.5</v>
@@ -3745,7 +3750,7 @@
         <v>1.5</v>
       </c>
       <c r="F145" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -3753,7 +3758,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C146">
         <v>1.5</v>
@@ -3765,7 +3770,7 @@
         <v>1.5</v>
       </c>
       <c r="F146" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>